<commit_message>
Update a_score views, templates, utils. Refactory admin_views and management commands
</commit_message>
<xml_diff>
--- a/a_predict/data/answer_official.xlsx
+++ b/a_predict/data/answer_official.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\paedison3\a_predict\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_predict\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E96867-45B9-4DEA-B9F5-CC0F49DFE0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565E7906-44D6-4DDC-A022-9BAAEF3F3786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="16800" windowHeight="15150" xr2:uid="{3A6622FD-35C9-421C-8813-00F77D8B68A4}"/>
+    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" xr2:uid="{3A6622FD-35C9-421C-8813-00F77D8B68A4}"/>
   </bookViews>
   <sheets>
     <sheet name="정답" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>no.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,10 @@
   </si>
   <si>
     <t>상황</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헌법</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -435,71 +439,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCD1352-56A8-46EC-877E-7C0163E40905}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -507,32 +523,38 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -540,148 +562,181 @@
       <c r="D7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -689,27 +744,33 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -717,41 +778,50 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -762,49 +832,271 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>